<commit_message>
update dac ta usecase 6/10/2019
</commit_message>
<xml_diff>
--- a/BaoCaoTienDo.xlsx
+++ b/BaoCaoTienDo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t xml:space="preserve">Tuần </t>
   </si>
@@ -92,15 +92,15 @@
     <t>Vẽ Sequence Diagram</t>
   </si>
   <si>
-    <t>Thiết kế giao diện</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 Sinh viên thực hiện:
 </t>
   </si>
   <si>
     <t>TS. Lê Văn Vinh</t>
+  </si>
+  <si>
+    <t>Đặc tả Usecase</t>
   </si>
 </sst>
 </file>
@@ -219,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -237,6 +237,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -248,15 +257,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,7 +541,7 @@
   <dimension ref="B1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F6" sqref="F6:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,11 +557,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="H1" s="5"/>
@@ -571,11 +572,11 @@
       <c r="M1" s="6"/>
     </row>
     <row r="2" spans="2:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="H2" s="5"/>
@@ -595,8 +596,8 @@
       <c r="D6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>19</v>
+      <c r="F6" s="13" t="s">
+        <v>18</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -606,7 +607,7 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -615,7 +616,7 @@
       <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="11"/>
+      <c r="F7" s="14"/>
       <c r="G7" s="2" t="s">
         <v>7</v>
       </c>
@@ -624,7 +625,7 @@
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="15"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
@@ -635,12 +636,12 @@
         <v>12</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="16"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
@@ -649,34 +650,40 @@
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="15"/>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="11"/>
+      <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="15"/>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B13" s="12"/>
+      <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="16"/>
-      <c r="C13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
@@ -687,24 +694,24 @@
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="15"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="15"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="16"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>

</xml_diff>